<commit_message>
Revised Project 1 margins and plot.
</commit_message>
<xml_diff>
--- a/Margins (Diss Projects 1-2).xlsx
+++ b/Margins (Diss Projects 1-2).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlb15b\Desktop\STATA Data\Dissertation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Desktop/School/Dissertation/Analyses:Results/R Project/Understanding_Resilience/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8066D97B-C983-4F58-9496-64FACE2A02BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABE9B27-803C-0543-BCE5-D9CF09547339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Margins (Project 1 Pars)" sheetId="1" r:id="rId1"/>
@@ -919,11 +919,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -946,7 +948,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -957,19 +959,19 @@
         <v>-2</v>
       </c>
       <c r="D2">
-        <v>2.9962979999999999</v>
+        <v>3.1647699999999999</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
       <c r="F2">
-        <v>2.9427439999999998</v>
+        <v>3.1105700000000001</v>
       </c>
       <c r="G2">
-        <v>3.0498530000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.218969</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -980,19 +982,19 @@
         <v>-2</v>
       </c>
       <c r="D3">
-        <v>2.9093249999999999</v>
+        <v>3.2918829999999999</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
       <c r="F3">
-        <v>2.7992219999999999</v>
+        <v>3.1932</v>
       </c>
       <c r="G3">
-        <v>3.019428</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.3905660000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1003,19 +1005,19 @@
         <v>-2</v>
       </c>
       <c r="D4">
-        <v>3.0221469999999999</v>
+        <v>3.2128830000000002</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4">
-        <v>2.8912580000000001</v>
+        <v>3.0644960000000001</v>
       </c>
       <c r="G4">
-        <v>3.1530360000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.3612709999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1026,19 +1028,19 @@
         <v>-1</v>
       </c>
       <c r="D5">
-        <v>3.284532</v>
+        <v>3.3466939999999998</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
       <c r="F5">
-        <v>3.248615</v>
+        <v>3.3110580000000001</v>
       </c>
       <c r="G5">
-        <v>3.3204479999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.3823300000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1049,19 +1051,19 @@
         <v>-1</v>
       </c>
       <c r="D6">
-        <v>3.120441</v>
+        <v>3.3808820000000002</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
       <c r="F6">
-        <v>3.0524450000000001</v>
+        <v>3.3204020000000001</v>
       </c>
       <c r="G6">
-        <v>3.188437</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.4413610000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1072,19 +1074,19 @@
         <v>-1</v>
       </c>
       <c r="D7">
-        <v>3.265682</v>
+        <v>3.369583</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="F7">
-        <v>3.1839279999999999</v>
+        <v>3.2792659999999998</v>
       </c>
       <c r="G7">
-        <v>3.3474349999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.4598990000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1095,19 +1097,19 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>3.572765</v>
+        <v>3.5286179999999998</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8">
-        <v>3.5461649999999998</v>
+        <v>3.5016750000000001</v>
       </c>
       <c r="G8">
-        <v>3.599364</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.5555599999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1118,19 +1120,19 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>3.3315579999999998</v>
+        <v>3.4698799999999999</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
       <c r="F9">
-        <v>3.2910970000000002</v>
+        <v>3.4311090000000002</v>
       </c>
       <c r="G9">
-        <v>3.3720180000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.508651</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1141,19 +1143,19 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>3.5092159999999999</v>
+        <v>3.5262820000000001</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
       </c>
       <c r="F10">
-        <v>3.4497149999999999</v>
+        <v>3.4638239999999998</v>
       </c>
       <c r="G10">
-        <v>3.5687180000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.58874</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1164,19 +1166,19 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>3.8609979999999999</v>
+        <v>3.7105419999999998</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
       </c>
       <c r="F11">
-        <v>3.8275190000000001</v>
+        <v>3.6744110000000001</v>
       </c>
       <c r="G11">
-        <v>3.894476</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.7466729999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1187,19 +1189,19 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>3.5426739999999999</v>
+        <v>3.558878</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
       </c>
       <c r="F12">
-        <v>3.4864299999999999</v>
+        <v>3.501655</v>
       </c>
       <c r="G12">
-        <v>3.5989179999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.616101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1210,19 +1212,19 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>3.7527509999999999</v>
+        <v>3.6829809999999998</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
       <c r="F13">
-        <v>3.664987</v>
+        <v>3.5868009999999999</v>
       </c>
       <c r="G13">
-        <v>3.8405140000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.7791619999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1233,19 +1235,19 @@
         <v>2</v>
       </c>
       <c r="D14">
-        <v>4.1492310000000003</v>
+        <v>3.8924660000000002</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
       </c>
       <c r="F14">
-        <v>4.0989339999999999</v>
+        <v>3.837615</v>
       </c>
       <c r="G14">
-        <v>4.1995279999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.947317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1256,19 +1258,19 @@
         <v>2</v>
       </c>
       <c r="D15">
-        <v>3.75379</v>
+        <v>3.6478769999999998</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
       </c>
       <c r="F15">
-        <v>3.657861</v>
+        <v>3.5531579999999998</v>
       </c>
       <c r="G15">
-        <v>3.84972</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.7425959999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1279,16 +1281,16 @@
         <v>2</v>
       </c>
       <c r="D16">
-        <v>3.9962849999999999</v>
+        <v>3.8396810000000001</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
       </c>
       <c r="F16">
-        <v>3.8578320000000001</v>
+        <v>3.6840980000000001</v>
       </c>
       <c r="G16">
-        <v>4.1347389999999997</v>
+        <v>3.995263</v>
       </c>
     </row>
   </sheetData>
@@ -1304,9 +1306,9 @@
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1335,7 +1337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1364,7 +1366,7 @@
         <v>3.495622</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1393,7 +1395,7 @@
         <v>3.4009429999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1422,7 +1424,7 @@
         <v>3.2396280000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1451,7 +1453,7 @@
         <v>3.6055679999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1480,7 +1482,7 @@
         <v>3.4815589999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1509,7 +1511,7 @@
         <v>3.45031</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1538,7 +1540,7 @@
         <v>3.7307329999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1567,7 +1569,7 @@
         <v>3.593324</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1596,7 +1598,7 @@
         <v>3.6946629999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1625,7 +1627,7 @@
         <v>3.8932280000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1654,7 +1656,7 @@
         <v>3.7864239999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1683,7 +1685,7 @@
         <v>4.0014250000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1712,7 +1714,7 @@
         <v>4.0739270000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1741,7 +1743,7 @@
         <v>4.0282900000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1770,7 +1772,7 @@
         <v>4.3509510000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1799,7 +1801,7 @@
         <v>3.098614</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1828,7 +1830,7 @@
         <v>3.2815500000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1857,7 +1859,7 @@
         <v>3.5160680000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1886,7 +1888,7 @@
         <v>3.2292800000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1915,7 +1917,7 @@
         <v>3.3216100000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1944,7 +1946,7 @@
         <v>3.5387140000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1973,7 +1975,7 @@
         <v>3.3928410000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2002,7 +2004,7 @@
         <v>3.3854880000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2031,7 +2033,7 @@
         <v>3.601817</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2060,7 +2062,7 @@
         <v>3.6029070000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2089,7 +2091,7 @@
         <v>3.5010409999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2118,7 +2120,7 @@
         <v>3.708129</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -2147,7 +2149,7 @@
         <v>3.8274919999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -2176,7 +2178,7 @@
         <v>3.6420370000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2219,9 +2221,9 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2250,7 +2252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2279,7 +2281,7 @@
         <v>3.4785309999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2308,7 +2310,7 @@
         <v>3.4297240000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2337,7 +2339,7 @@
         <v>3.3513380000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2366,7 +2368,7 @@
         <v>3.5924939999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2395,7 +2397,7 @@
         <v>3.4795310000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2424,7 +2426,7 @@
         <v>3.5034169999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2453,7 +2455,7 @@
         <v>3.725876</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2482,7 +2484,7 @@
         <v>3.5752989999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2511,7 +2513,7 @@
         <v>3.710788</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2540,7 +2542,7 @@
         <v>3.888833</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2569,7 +2571,7 @@
         <v>3.7523339999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2598,7 +2600,7 @@
         <v>4.0105399999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2627,7 +2629,7 @@
         <v>4.0633280000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2656,7 +2658,7 @@
         <v>3.9698669999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2685,7 +2687,7 @@
         <v>4.3524630000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -2714,7 +2716,7 @@
         <v>3.0613999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2743,7 +2745,7 @@
         <v>3.242162</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -2772,7 +2774,7 @@
         <v>3.484712</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -2801,7 +2803,7 @@
         <v>3.196196</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -2830,7 +2832,7 @@
         <v>3.3130630000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -2859,7 +2861,7 @@
         <v>3.528397</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -2888,7 +2890,7 @@
         <v>3.3853490000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2917,7 +2919,7 @@
         <v>3.4018280000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2946,7 +2948,7 @@
         <v>3.6045199999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2975,7 +2977,7 @@
         <v>3.6385510000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3004,7 +3006,7 @@
         <v>3.5347499999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3033,7 +3035,7 @@
         <v>3.724405</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -3062,7 +3064,7 @@
         <v>3.9042759999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -3091,7 +3093,7 @@
         <v>3.690725</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -3131,9 +3133,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3162,7 +3164,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3191,7 +3193,7 @@
         <v>3.428112</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3220,7 +3222,7 @@
         <v>3.313097</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3249,7 +3251,7 @@
         <v>3.335261</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3278,7 +3280,7 @@
         <v>3.555291</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3307,7 +3309,7 @@
         <v>3.4164970000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3336,7 +3338,7 @@
         <v>3.498256</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3365,7 +3367,7 @@
         <v>3.6963270000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3394,7 +3396,7 @@
         <v>3.5446659999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -3423,7 +3425,7 @@
         <v>3.6822940000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3452,7 +3454,7 @@
         <v>3.8781180000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3481,7 +3483,7 @@
         <v>3.734076</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3510,7 +3512,7 @@
         <v>3.9244979999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -3539,7 +3541,7 @@
         <v>4.0831239999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3568,7 +3570,7 @@
         <v>3.9580129999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3597,7 +3599,7 @@
         <v>4.2242240000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -3626,7 +3628,7 @@
         <v>3.1884570000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3655,7 +3657,7 @@
         <v>3.3287</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -3684,7 +3686,7 @@
         <v>3.5510269999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -3713,7 +3715,7 @@
         <v>3.3188710000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -3742,7 +3744,7 @@
         <v>3.339299</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -3771,7 +3773,7 @@
         <v>3.5572629999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -3800,7 +3802,7 @@
         <v>3.4697650000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3829,7 +3831,7 @@
         <v>3.3818139999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -3858,7 +3860,7 @@
         <v>3.6126529999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -3887,7 +3889,7 @@
         <v>3.6514820000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3916,7 +3918,7 @@
         <v>3.4825149999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3945,7 +3947,7 @@
         <v>3.725654</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -3974,7 +3976,7 @@
         <v>3.8468969999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -4003,7 +4005,7 @@
         <v>3.6107619999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Revised Project 1 Margins and Plots.
</commit_message>
<xml_diff>
--- a/Margins (Diss Projects 1-2).xlsx
+++ b/Margins (Diss Projects 1-2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Desktop/School/Dissertation/Analyses:Results/R Project/Understanding_Resilience/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABE9B27-803C-0543-BCE5-D9CF09547339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AD2275-8597-8F4C-AA02-4E678FA440CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Margins (Project 1 Pars)" sheetId="1" r:id="rId1"/>
@@ -920,7 +920,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -959,16 +959,16 @@
         <v>-2</v>
       </c>
       <c r="D2">
-        <v>3.1647699999999999</v>
+        <v>3.3075009999999998</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
       <c r="F2">
-        <v>3.1105700000000001</v>
+        <v>3.2543859999999998</v>
       </c>
       <c r="G2">
-        <v>3.218969</v>
+        <v>3.360617</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -982,16 +982,16 @@
         <v>-2</v>
       </c>
       <c r="D3">
-        <v>3.2918829999999999</v>
+        <v>3.4236140000000002</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F3">
-        <v>3.1932</v>
+        <v>3.3363070000000001</v>
       </c>
       <c r="G3">
-        <v>3.3905660000000002</v>
+        <v>3.5109210000000002</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1005,16 +1005,16 @@
         <v>-2</v>
       </c>
       <c r="D4">
-        <v>3.2128830000000002</v>
+        <v>3.3906540000000001</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4">
-        <v>3.0644960000000001</v>
+        <v>3.2583440000000001</v>
       </c>
       <c r="G4">
-        <v>3.3612709999999999</v>
+        <v>3.5229629999999998</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1028,16 +1028,16 @@
         <v>-1</v>
       </c>
       <c r="D5">
-        <v>3.3466939999999998</v>
+        <v>3.4118170000000001</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
       <c r="F5">
-        <v>3.3110580000000001</v>
+        <v>3.3758189999999999</v>
       </c>
       <c r="G5">
-        <v>3.3823300000000001</v>
+        <v>3.447816</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1051,16 +1051,16 @@
         <v>-1</v>
       </c>
       <c r="D6">
-        <v>3.3808820000000002</v>
+        <v>3.4547780000000001</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F6">
-        <v>3.3204020000000001</v>
+        <v>3.3970009999999999</v>
       </c>
       <c r="G6">
-        <v>3.4413610000000001</v>
+        <v>3.5125549999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1074,16 +1074,16 @@
         <v>-1</v>
       </c>
       <c r="D7">
-        <v>3.369583</v>
+        <v>3.47167</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="F7">
-        <v>3.2792659999999998</v>
+        <v>3.389154</v>
       </c>
       <c r="G7">
-        <v>3.4598990000000001</v>
+        <v>3.5541849999999999</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1097,16 +1097,16 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>3.5286179999999998</v>
+        <v>3.516133</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8">
-        <v>3.5016750000000001</v>
+        <v>3.4890840000000001</v>
       </c>
       <c r="G8">
-        <v>3.5555599999999998</v>
+        <v>3.543183</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1120,16 +1120,16 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>3.4698799999999999</v>
+        <v>3.4859420000000001</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F9">
-        <v>3.4311090000000002</v>
+        <v>3.4460709999999999</v>
       </c>
       <c r="G9">
-        <v>3.508651</v>
+        <v>3.5258129999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1143,16 +1143,16 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>3.5262820000000001</v>
+        <v>3.5526849999999999</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
       </c>
       <c r="F10">
-        <v>3.4638239999999998</v>
+        <v>3.493458</v>
       </c>
       <c r="G10">
-        <v>3.58874</v>
+        <v>3.6119129999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1166,16 +1166,16 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>3.7105419999999998</v>
+        <v>3.6204489999999998</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
       </c>
       <c r="F11">
-        <v>3.6744110000000001</v>
+        <v>3.586856</v>
       </c>
       <c r="G11">
-        <v>3.7466729999999999</v>
+        <v>3.6540430000000002</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1189,16 +1189,16 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>3.558878</v>
+        <v>3.5171060000000001</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F12">
-        <v>3.501655</v>
+        <v>3.4683519999999999</v>
       </c>
       <c r="G12">
-        <v>3.616101</v>
+        <v>3.5658599999999998</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1212,16 +1212,16 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>3.6829809999999998</v>
+        <v>3.6337009999999998</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
       <c r="F13">
-        <v>3.5868009999999999</v>
+        <v>3.5465059999999999</v>
       </c>
       <c r="G13">
-        <v>3.7791619999999999</v>
+        <v>3.7208969999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1235,16 +1235,16 @@
         <v>2</v>
       </c>
       <c r="D14">
-        <v>3.8924660000000002</v>
+        <v>3.7247650000000001</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
       </c>
       <c r="F14">
-        <v>3.837615</v>
+        <v>3.6749010000000002</v>
       </c>
       <c r="G14">
-        <v>3.947317</v>
+        <v>3.7746300000000002</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1258,16 +1258,16 @@
         <v>2</v>
       </c>
       <c r="D15">
-        <v>3.6478769999999998</v>
+        <v>3.54827</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F15">
-        <v>3.5531579999999998</v>
+        <v>3.4727709999999998</v>
       </c>
       <c r="G15">
-        <v>3.7425959999999998</v>
+        <v>3.6237689999999998</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1281,16 +1281,16 @@
         <v>2</v>
       </c>
       <c r="D16">
-        <v>3.8396810000000001</v>
+        <v>3.7147169999999998</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
       </c>
       <c r="F16">
-        <v>3.6840980000000001</v>
+        <v>3.5765349999999998</v>
       </c>
       <c r="G16">
-        <v>3.995263</v>
+        <v>3.8528989999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Confidence Intervals from 80% to 84%
</commit_message>
<xml_diff>
--- a/Margins (Diss Projects 1-2).xlsx
+++ b/Margins (Diss Projects 1-2).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Desktop/School/Dissertation/Analyses:Results/R Project/Understanding_Resilience/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlb15b\Desktop\STATA Data\Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AD2275-8597-8F4C-AA02-4E678FA440CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530E1267-A25F-4101-84A0-6BF4F924F22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Margins (Project 1 Pars)" sheetId="1" r:id="rId1"/>
@@ -919,13 +919,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H34" sqref="C19:H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -948,7 +948,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -965,13 +965,13 @@
         <v>11</v>
       </c>
       <c r="F2">
-        <v>3.2543859999999998</v>
+        <v>3.249225</v>
       </c>
       <c r="G2">
-        <v>3.360617</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.3657780000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -988,13 +988,13 @@
         <v>15</v>
       </c>
       <c r="F3">
-        <v>3.3363070000000001</v>
+        <v>3.327823</v>
       </c>
       <c r="G3">
-        <v>3.5109210000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.5194049999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1011,13 +1011,13 @@
         <v>11</v>
       </c>
       <c r="F4">
-        <v>3.2583440000000001</v>
+        <v>3.2454860000000001</v>
       </c>
       <c r="G4">
-        <v>3.5229629999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.5358209999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1034,13 +1034,13 @@
         <v>11</v>
       </c>
       <c r="F5">
-        <v>3.3758189999999999</v>
+        <v>3.3723209999999999</v>
       </c>
       <c r="G5">
-        <v>3.447816</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.451314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1057,13 +1057,13 @@
         <v>15</v>
       </c>
       <c r="F6">
-        <v>3.3970009999999999</v>
+        <v>3.3913869999999999</v>
       </c>
       <c r="G6">
-        <v>3.5125549999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.5181689999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1080,13 +1080,13 @@
         <v>11</v>
       </c>
       <c r="F7">
-        <v>3.389154</v>
+        <v>3.381135</v>
       </c>
       <c r="G7">
-        <v>3.5541849999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.5622039999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1103,13 +1103,13 @@
         <v>11</v>
       </c>
       <c r="F8">
-        <v>3.4890840000000001</v>
+        <v>3.486456</v>
       </c>
       <c r="G8">
-        <v>3.543183</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.545811</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1126,13 +1126,13 @@
         <v>15</v>
       </c>
       <c r="F9">
-        <v>3.4460709999999999</v>
+        <v>3.4421970000000002</v>
       </c>
       <c r="G9">
-        <v>3.5258129999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.529687</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1149,13 +1149,13 @@
         <v>11</v>
       </c>
       <c r="F10">
-        <v>3.493458</v>
+        <v>3.4877030000000002</v>
       </c>
       <c r="G10">
-        <v>3.6119129999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.6176680000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1172,13 +1172,13 @@
         <v>11</v>
       </c>
       <c r="F11">
-        <v>3.586856</v>
+        <v>3.5835919999999999</v>
       </c>
       <c r="G11">
-        <v>3.6540430000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.6573069999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1195,13 +1195,13 @@
         <v>15</v>
       </c>
       <c r="F12">
-        <v>3.4683519999999999</v>
+        <v>3.4636140000000002</v>
       </c>
       <c r="G12">
-        <v>3.5658599999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.5705979999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1218,13 +1218,13 @@
         <v>11</v>
       </c>
       <c r="F13">
-        <v>3.5465059999999999</v>
+        <v>3.538033</v>
       </c>
       <c r="G13">
-        <v>3.7208969999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.7293690000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1241,13 +1241,13 @@
         <v>11</v>
       </c>
       <c r="F14">
-        <v>3.6749010000000002</v>
+        <v>3.6700550000000001</v>
       </c>
       <c r="G14">
-        <v>3.7746300000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.7794759999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1264,13 +1264,13 @@
         <v>15</v>
       </c>
       <c r="F15">
-        <v>3.4727709999999998</v>
+        <v>3.4654349999999998</v>
       </c>
       <c r="G15">
-        <v>3.6237689999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.6311049999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1287,10 +1287,10 @@
         <v>11</v>
       </c>
       <c r="F16">
-        <v>3.5765349999999998</v>
+        <v>3.5631080000000002</v>
       </c>
       <c r="G16">
-        <v>3.8528989999999999</v>
+        <v>3.8663259999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1303,12 +1303,12 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1360,13 +1360,13 @@
         <v>11</v>
       </c>
       <c r="H2">
-        <v>3.30925</v>
+        <v>3.300195</v>
       </c>
       <c r="I2">
-        <v>3.495622</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.504677</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1389,13 +1389,13 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <v>2.9414359999999999</v>
+        <v>2.9191099999999999</v>
       </c>
       <c r="I3">
-        <v>3.4009429999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4232689999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1418,13 +1418,13 @@
         <v>11</v>
       </c>
       <c r="H4">
-        <v>2.764929</v>
+        <v>2.7418529999999999</v>
       </c>
       <c r="I4">
-        <v>3.2396280000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.262705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1447,13 +1447,13 @@
         <v>11</v>
       </c>
       <c r="H5">
-        <v>3.490796</v>
+        <v>3.48522</v>
       </c>
       <c r="I5">
-        <v>3.6055679999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6111439999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1476,13 +1476,13 @@
         <v>11</v>
       </c>
       <c r="H6">
-        <v>3.1891829999999999</v>
+        <v>3.1749770000000002</v>
       </c>
       <c r="I6">
-        <v>3.4815589999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.495765</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1505,13 +1505,13 @@
         <v>11</v>
       </c>
       <c r="H7">
-        <v>3.1202450000000002</v>
+        <v>3.104203</v>
       </c>
       <c r="I7">
-        <v>3.45031</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4663520000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1534,13 +1534,13 @@
         <v>11</v>
       </c>
       <c r="H8">
-        <v>3.6571229999999999</v>
+        <v>3.6535470000000001</v>
       </c>
       <c r="I8">
-        <v>3.7307329999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.7343090000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1563,13 +1563,13 @@
         <v>11</v>
       </c>
       <c r="H9">
-        <v>3.4057810000000002</v>
+        <v>3.3966690000000002</v>
       </c>
       <c r="I9">
-        <v>3.593324</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.602436</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1592,13 +1592,13 @@
         <v>11</v>
       </c>
       <c r="H10">
-        <v>3.4418890000000002</v>
+        <v>3.429608</v>
       </c>
       <c r="I10">
-        <v>3.6946629999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.706944</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1621,13 +1621,13 @@
         <v>11</v>
       </c>
       <c r="H11">
-        <v>3.7861199999999999</v>
+        <v>3.7809159999999999</v>
       </c>
       <c r="I11">
-        <v>3.8932280000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.8984320000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1650,13 +1650,13 @@
         <v>11</v>
       </c>
       <c r="H12">
-        <v>3.5410439999999999</v>
+        <v>3.5291220000000001</v>
       </c>
       <c r="I12">
-        <v>3.7864239999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.798346</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1679,13 +1679,13 @@
         <v>11</v>
       </c>
       <c r="H13">
-        <v>3.7011240000000001</v>
+        <v>3.686534</v>
       </c>
       <c r="I13">
-        <v>4.0014250000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0160150000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1708,13 +1708,13 @@
         <v>11</v>
       </c>
       <c r="H14">
-        <v>3.8969130000000001</v>
+        <v>3.8883130000000001</v>
       </c>
       <c r="I14">
-        <v>4.0739270000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0825269999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1737,13 +1737,13 @@
         <v>11</v>
       </c>
       <c r="H15">
-        <v>3.6275409999999999</v>
+        <v>3.6080700000000001</v>
       </c>
       <c r="I15">
-        <v>4.0282900000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0477610000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1766,13 +1766,13 @@
         <v>11</v>
       </c>
       <c r="H16">
-        <v>3.9175949999999999</v>
+        <v>3.8965360000000002</v>
       </c>
       <c r="I16">
-        <v>4.3509510000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.3720100000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1795,13 +1795,13 @@
         <v>11</v>
       </c>
       <c r="H17">
-        <v>2.882285</v>
+        <v>2.8717739999999998</v>
       </c>
       <c r="I17">
-        <v>3.098614</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.109124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1824,13 +1824,13 @@
         <v>15</v>
       </c>
       <c r="H18">
-        <v>3.0097809999999998</v>
+        <v>2.9965769999999998</v>
       </c>
       <c r="I18">
-        <v>3.2815500000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.2947540000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1853,13 +1853,13 @@
         <v>15</v>
       </c>
       <c r="H19">
-        <v>3.2473649999999998</v>
+        <v>3.2343060000000001</v>
       </c>
       <c r="I19">
-        <v>3.5160680000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5291269999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1882,13 +1882,13 @@
         <v>11</v>
       </c>
       <c r="H20">
-        <v>3.1011700000000002</v>
+        <v>3.0949450000000001</v>
       </c>
       <c r="I20">
-        <v>3.2292800000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.2355040000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1911,13 +1911,13 @@
         <v>15</v>
       </c>
       <c r="H21">
-        <v>3.1513179999999998</v>
+        <v>3.1430449999999999</v>
       </c>
       <c r="I21">
-        <v>3.3216100000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3298830000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1940,13 +1940,13 @@
         <v>15</v>
       </c>
       <c r="H22">
-        <v>3.3566859999999998</v>
+        <v>3.347839</v>
       </c>
       <c r="I22">
-        <v>3.5387140000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.547561</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1969,13 +1969,13 @@
         <v>11</v>
       </c>
       <c r="H23">
-        <v>3.2871600000000001</v>
+        <v>3.282025</v>
       </c>
       <c r="I23">
-        <v>3.3928410000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3979759999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1998,13 +1998,13 @@
         <v>15</v>
       </c>
       <c r="H24">
-        <v>3.269037</v>
+        <v>3.2633800000000002</v>
       </c>
       <c r="I24">
-        <v>3.3854880000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3911449999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2027,13 +2027,13 @@
         <v>15</v>
       </c>
       <c r="H25">
-        <v>3.4255499999999999</v>
+        <v>3.4169860000000001</v>
       </c>
       <c r="I25">
-        <v>3.601817</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6103809999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2056,13 +2056,13 @@
         <v>11</v>
       </c>
       <c r="H26">
-        <v>3.4266450000000002</v>
+        <v>3.4180820000000001</v>
       </c>
       <c r="I26">
-        <v>3.6029070000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6114700000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2085,13 +2085,13 @@
         <v>15</v>
       </c>
       <c r="H27">
-        <v>3.3350810000000002</v>
+        <v>3.3270179999999998</v>
       </c>
       <c r="I27">
-        <v>3.5010409999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5091039999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2114,13 +2114,13 @@
         <v>15</v>
       </c>
       <c r="H28">
-        <v>3.4512049999999999</v>
+        <v>3.438723</v>
       </c>
       <c r="I28">
-        <v>3.708129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.7206109999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -2143,13 +2143,13 @@
         <v>11</v>
       </c>
       <c r="H29">
-        <v>3.5516109999999999</v>
+        <v>3.538208</v>
       </c>
       <c r="I29">
-        <v>3.8274919999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.8408959999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -2172,13 +2172,13 @@
         <v>15</v>
       </c>
       <c r="H30">
-        <v>3.3756819999999998</v>
+        <v>3.3627410000000002</v>
       </c>
       <c r="I30">
-        <v>3.6420370000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6549779999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2201,10 +2201,10 @@
         <v>15</v>
       </c>
       <c r="H31">
-        <v>3.4599410000000002</v>
+        <v>3.441897</v>
       </c>
       <c r="I31">
-        <v>3.8313600000000001</v>
+        <v>3.849405</v>
       </c>
     </row>
   </sheetData>
@@ -2217,13 +2217,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6B9039-CBE8-49C0-9D0B-FD71EAE35EE3}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2275,13 +2275,13 @@
         <v>11</v>
       </c>
       <c r="H2">
-        <v>3.3253189999999999</v>
+        <v>3.3178749999999999</v>
       </c>
       <c r="I2">
-        <v>3.4785309999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4859749999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2304,13 +2304,13 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <v>2.9580479999999998</v>
+        <v>2.9351289999999999</v>
       </c>
       <c r="I3">
-        <v>3.4297240000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4526430000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2333,13 +2333,13 @@
         <v>11</v>
       </c>
       <c r="H4">
-        <v>2.8370790000000001</v>
+        <v>2.8120790000000002</v>
       </c>
       <c r="I4">
-        <v>3.3513380000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3763380000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2362,13 +2362,13 @@
         <v>11</v>
       </c>
       <c r="H5">
-        <v>3.4968189999999999</v>
+        <v>3.4921700000000002</v>
       </c>
       <c r="I5">
-        <v>3.5924939999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5971419999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2391,13 +2391,13 @@
         <v>11</v>
       </c>
       <c r="H6">
-        <v>3.1731980000000002</v>
+        <v>3.1583130000000001</v>
       </c>
       <c r="I6">
-        <v>3.4795310000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4944160000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2420,13 +2420,13 @@
         <v>11</v>
       </c>
       <c r="H7">
-        <v>3.1735259999999998</v>
+        <v>3.1574900000000001</v>
       </c>
       <c r="I7">
-        <v>3.5034169999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5194540000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2449,13 +2449,13 @@
         <v>11</v>
       </c>
       <c r="H8">
-        <v>3.6488990000000001</v>
+        <v>3.645159</v>
       </c>
       <c r="I8">
-        <v>3.725876</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.729616</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2478,13 +2478,13 @@
         <v>11</v>
       </c>
       <c r="H9">
-        <v>3.342387</v>
+        <v>3.3310710000000001</v>
       </c>
       <c r="I9">
-        <v>3.5752989999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5866150000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2507,13 +2507,13 @@
         <v>11</v>
       </c>
       <c r="H10">
-        <v>3.454682</v>
+        <v>3.442237</v>
       </c>
       <c r="I10">
-        <v>3.710788</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.723233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2536,13 +2536,13 @@
         <v>11</v>
       </c>
       <c r="H11">
-        <v>3.7714050000000001</v>
+        <v>3.7656999999999998</v>
       </c>
       <c r="I11">
-        <v>3.888833</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.8945379999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2565,13 +2565,13 @@
         <v>11</v>
       </c>
       <c r="H12">
-        <v>3.4303089999999998</v>
+        <v>3.414663</v>
       </c>
       <c r="I12">
-        <v>3.7523339999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.7679800000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2594,13 +2594,13 @@
         <v>11</v>
       </c>
       <c r="H13">
-        <v>3.643456</v>
+        <v>3.6256210000000002</v>
       </c>
       <c r="I13">
-        <v>4.0105399999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0283759999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2623,13 +2623,13 @@
         <v>11</v>
       </c>
       <c r="H14">
-        <v>3.8823729999999999</v>
+        <v>3.8735810000000002</v>
       </c>
       <c r="I14">
-        <v>4.0633280000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.07212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2652,13 +2652,13 @@
         <v>11</v>
       </c>
       <c r="H15">
-        <v>3.477732</v>
+        <v>3.4538199999999999</v>
       </c>
       <c r="I15">
-        <v>3.9698669999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.993779</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2681,13 +2681,13 @@
         <v>11</v>
       </c>
       <c r="H16">
-        <v>3.79006</v>
+        <v>3.7627329999999999</v>
       </c>
       <c r="I16">
-        <v>4.3524630000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.3797899999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -2710,13 +2710,13 @@
         <v>11</v>
       </c>
       <c r="H17">
-        <v>2.8041149999999999</v>
+        <v>2.7916150000000002</v>
       </c>
       <c r="I17">
-        <v>3.0613999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.0739000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2739,13 +2739,13 @@
         <v>15</v>
       </c>
       <c r="H18">
-        <v>3.0118770000000001</v>
+        <v>3.0006879999999998</v>
       </c>
       <c r="I18">
-        <v>3.242162</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.2533500000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -2768,13 +2768,13 @@
         <v>15</v>
       </c>
       <c r="H19">
-        <v>3.1951420000000001</v>
+        <v>3.1810700000000001</v>
       </c>
       <c r="I19">
-        <v>3.484712</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4987840000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -2797,13 +2797,13 @@
         <v>11</v>
       </c>
       <c r="H20">
-        <v>3.0610919999999999</v>
+        <v>3.0545279999999999</v>
       </c>
       <c r="I20">
-        <v>3.196196</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.2027610000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -2826,13 +2826,13 @@
         <v>15</v>
       </c>
       <c r="H21">
-        <v>3.169432</v>
+        <v>3.1624530000000002</v>
       </c>
       <c r="I21">
-        <v>3.3130630000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3200409999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -2855,13 +2855,13 @@
         <v>15</v>
       </c>
       <c r="H22">
-        <v>3.329653</v>
+        <v>3.319995</v>
       </c>
       <c r="I22">
-        <v>3.528397</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5380549999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -2884,13 +2884,13 @@
         <v>11</v>
       </c>
       <c r="H23">
-        <v>3.2637119999999999</v>
+        <v>3.2578019999999999</v>
       </c>
       <c r="I23">
-        <v>3.3853490000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3912589999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2913,13 +2913,13 @@
         <v>15</v>
       </c>
       <c r="H24">
-        <v>3.309123</v>
+        <v>3.3046180000000001</v>
       </c>
       <c r="I24">
-        <v>3.4018280000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4063319999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2942,13 +2942,13 @@
         <v>15</v>
       </c>
       <c r="H25">
-        <v>3.4317250000000001</v>
+        <v>3.4233289999999998</v>
       </c>
       <c r="I25">
-        <v>3.6045199999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6129159999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2971,13 +2971,13 @@
         <v>11</v>
       </c>
       <c r="H26">
-        <v>3.4022830000000002</v>
+        <v>3.3908040000000002</v>
       </c>
       <c r="I26">
-        <v>3.6385510000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6500300000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3000,13 +3000,13 @@
         <v>15</v>
       </c>
       <c r="H27">
-        <v>3.4046560000000001</v>
+        <v>3.3983349999999999</v>
       </c>
       <c r="I27">
-        <v>3.5347499999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5410710000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3029,13 +3029,13 @@
         <v>15</v>
       </c>
       <c r="H28">
-        <v>3.4900350000000002</v>
+        <v>3.4786480000000002</v>
       </c>
       <c r="I28">
-        <v>3.724405</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.735792</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -3058,13 +3058,13 @@
         <v>11</v>
       </c>
       <c r="H29">
-        <v>3.5283310000000001</v>
+        <v>3.5100660000000001</v>
       </c>
       <c r="I29">
-        <v>3.9042759999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.9225409999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -3087,13 +3087,13 @@
         <v>15</v>
       </c>
       <c r="H30">
-        <v>3.4771369999999999</v>
+        <v>3.4667590000000001</v>
       </c>
       <c r="I30">
-        <v>3.690725</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.7011029999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -3116,10 +3116,10 @@
         <v>15</v>
       </c>
       <c r="H31">
-        <v>3.5269729999999999</v>
+        <v>3.5105179999999998</v>
       </c>
       <c r="I31">
-        <v>3.8656630000000001</v>
+        <v>3.8821180000000002</v>
       </c>
     </row>
   </sheetData>
@@ -3131,11 +3131,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFB957D-785C-4A54-8A36-EE5236BB7762}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3164,7 +3166,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3187,13 +3189,13 @@
         <v>11</v>
       </c>
       <c r="H2">
-        <v>3.2156509999999998</v>
+        <v>3.2053289999999999</v>
       </c>
       <c r="I2">
-        <v>3.428112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.438434</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3216,13 +3218,13 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <v>2.975562</v>
+        <v>2.9591630000000002</v>
       </c>
       <c r="I3">
-        <v>3.313097</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3294969999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3245,13 +3247,13 @@
         <v>11</v>
       </c>
       <c r="H4">
-        <v>2.8315610000000002</v>
+        <v>2.807077</v>
       </c>
       <c r="I4">
-        <v>3.335261</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3597459999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3274,13 +3276,13 @@
         <v>11</v>
       </c>
       <c r="H5">
-        <v>3.4232040000000001</v>
+        <v>3.4167860000000001</v>
       </c>
       <c r="I5">
-        <v>3.555291</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.561709</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3303,13 +3305,13 @@
         <v>11</v>
       </c>
       <c r="H6">
-        <v>3.2027459999999999</v>
+        <v>3.192361</v>
       </c>
       <c r="I6">
-        <v>3.4164970000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4268830000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3332,13 +3334,13 @@
         <v>11</v>
       </c>
       <c r="H7">
-        <v>3.1516999999999999</v>
+        <v>3.1348560000000001</v>
       </c>
       <c r="I7">
-        <v>3.498256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5150999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3361,13 +3363,13 @@
         <v>11</v>
       </c>
       <c r="H8">
-        <v>3.6169009999999999</v>
+        <v>3.6130420000000001</v>
       </c>
       <c r="I8">
-        <v>3.6963270000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.700186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3390,13 +3392,13 @@
         <v>11</v>
       </c>
       <c r="H9">
-        <v>3.4051619999999998</v>
+        <v>3.3983840000000001</v>
       </c>
       <c r="I9">
-        <v>3.5446659999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.551444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -3419,13 +3421,13 @@
         <v>11</v>
       </c>
       <c r="H10">
-        <v>3.450793</v>
+        <v>3.4395449999999999</v>
       </c>
       <c r="I10">
-        <v>3.6822940000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.693543</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3448,13 +3450,13 @@
         <v>11</v>
       </c>
       <c r="H11">
-        <v>3.769841</v>
+        <v>3.7645810000000002</v>
       </c>
       <c r="I11">
-        <v>3.8781180000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.8833790000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3477,13 +3479,13 @@
         <v>11</v>
       </c>
       <c r="H12">
-        <v>3.5463369999999999</v>
+        <v>3.5372150000000002</v>
       </c>
       <c r="I12">
-        <v>3.734076</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.7431969999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3506,13 +3508,13 @@
         <v>11</v>
       </c>
       <c r="H13">
-        <v>3.6917230000000001</v>
+        <v>3.6804139999999999</v>
       </c>
       <c r="I13">
-        <v>3.9244979999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.9358070000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -3535,13 +3537,13 @@
         <v>11</v>
       </c>
       <c r="H14">
-        <v>3.8995669999999998</v>
+        <v>3.8906489999999998</v>
       </c>
       <c r="I14">
-        <v>4.0831239999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0920420000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3564,13 +3566,13 @@
         <v>11</v>
       </c>
       <c r="H15">
-        <v>3.652984</v>
+        <v>3.6381640000000002</v>
       </c>
       <c r="I15">
-        <v>3.9580129999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.9728330000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3593,13 +3595,13 @@
         <v>11</v>
       </c>
       <c r="H16">
-        <v>3.8751289999999998</v>
+        <v>3.8581650000000001</v>
       </c>
       <c r="I16">
-        <v>4.2242240000000004</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.2411880000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -3622,13 +3624,13 @@
         <v>11</v>
       </c>
       <c r="H17">
-        <v>3.0117340000000001</v>
+        <v>3.0031479999999999</v>
       </c>
       <c r="I17">
-        <v>3.1884570000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.197044</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3651,13 +3653,13 @@
         <v>15</v>
       </c>
       <c r="H18">
-        <v>3.0087739999999998</v>
+        <v>2.9932310000000002</v>
       </c>
       <c r="I18">
-        <v>3.3287</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3442430000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -3680,13 +3682,13 @@
         <v>15</v>
       </c>
       <c r="H19">
-        <v>3.2239599999999999</v>
+        <v>3.2080609999999998</v>
       </c>
       <c r="I19">
-        <v>3.5510269999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.566926</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -3709,13 +3711,13 @@
         <v>11</v>
       </c>
       <c r="H20">
-        <v>3.2040329999999999</v>
+        <v>3.1984530000000002</v>
       </c>
       <c r="I20">
-        <v>3.3188710000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3244509999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -3738,13 +3740,13 @@
         <v>15</v>
       </c>
       <c r="H21">
-        <v>3.1353059999999999</v>
+        <v>3.1253950000000001</v>
       </c>
       <c r="I21">
-        <v>3.339299</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3492099999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -3767,13 +3769,13 @@
         <v>15</v>
       </c>
       <c r="H22">
-        <v>3.3449080000000002</v>
+        <v>3.3345850000000001</v>
       </c>
       <c r="I22">
-        <v>3.5572629999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5675870000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -3796,13 +3798,13 @@
         <v>11</v>
       </c>
       <c r="H23">
-        <v>3.3758509999999999</v>
+        <v>3.371289</v>
       </c>
       <c r="I23">
-        <v>3.4697650000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4743270000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3825,13 +3827,13 @@
         <v>15</v>
       </c>
       <c r="H24">
-        <v>3.2299220000000002</v>
+        <v>3.2225429999999999</v>
       </c>
       <c r="I24">
-        <v>3.3818139999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3891930000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -3854,13 +3856,13 @@
         <v>15</v>
       </c>
       <c r="H25">
-        <v>3.4167040000000002</v>
+        <v>3.4071829999999999</v>
       </c>
       <c r="I25">
-        <v>3.6126529999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6221739999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -3883,13 +3885,13 @@
         <v>11</v>
       </c>
       <c r="H26">
-        <v>3.5168469999999998</v>
+        <v>3.5103059999999999</v>
       </c>
       <c r="I26">
-        <v>3.6514820000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.658023</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3912,13 +3914,13 @@
         <v>15</v>
       </c>
       <c r="H27">
-        <v>3.2663530000000001</v>
+        <v>3.2558509999999998</v>
       </c>
       <c r="I27">
-        <v>3.4825149999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.493017</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3941,13 +3943,13 @@
         <v>15</v>
       </c>
       <c r="H28">
-        <v>3.4308879999999999</v>
+        <v>3.4165670000000001</v>
       </c>
       <c r="I28">
-        <v>3.725654</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.7399740000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -3970,13 +3972,13 @@
         <v>11</v>
       </c>
       <c r="H29">
-        <v>3.6441439999999998</v>
+        <v>3.6342940000000001</v>
       </c>
       <c r="I29">
-        <v>3.8468969999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.8567469999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -3999,13 +4001,13 @@
         <v>15</v>
       </c>
       <c r="H30">
-        <v>3.275236</v>
+        <v>3.2589350000000001</v>
       </c>
       <c r="I30">
-        <v>3.6107619999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6270639999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -4028,10 +4030,10 @@
         <v>15</v>
       </c>
       <c r="H31">
-        <v>3.4235980000000001</v>
+        <v>3.40239</v>
       </c>
       <c r="I31">
-        <v>3.860128</v>
+        <v>3.8813360000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Estimates of Disadvantage by Race
</commit_message>
<xml_diff>
--- a/Margins (Diss Projects 1-2).xlsx
+++ b/Margins (Diss Projects 1-2).xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Desktop/School/Dissertation/Analyses:Results/R Project/Understanding_Resilience/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlb15b\Desktop\STATA Data\Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06783DC-49B5-4E44-B766-143E25324D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6922B16A-B992-4F8B-A02B-7D089CE9F30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Margins (Project 1 Pars)" sheetId="1" r:id="rId1"/>
-    <sheet name="Margins (Total Disad)" sheetId="2" r:id="rId2"/>
-    <sheet name="Margins (Material Disad)" sheetId="3" r:id="rId3"/>
-    <sheet name="Margins (Social Disad)" sheetId="4" r:id="rId4"/>
+    <sheet name="Disadvantage by Race (Desc)" sheetId="5" r:id="rId1"/>
+    <sheet name="Margins (Project 1 Pars)" sheetId="1" r:id="rId2"/>
+    <sheet name="Margins (Total Disad)" sheetId="2" r:id="rId3"/>
+    <sheet name="Margins (Material Disad)" sheetId="3" r:id="rId4"/>
+    <sheet name="Margins (Social Disad)" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="25">
   <si>
     <t>race_eth</t>
   </si>
@@ -71,6 +72,33 @@
   </si>
   <si>
     <t>NS</t>
+  </si>
+  <si>
+    <t>disad_mean</t>
+  </si>
+  <si>
+    <t>disad_type</t>
+  </si>
+  <si>
+    <t>disad_type_q</t>
+  </si>
+  <si>
+    <t>socdisad_f</t>
+  </si>
+  <si>
+    <t>matdisad_f</t>
+  </si>
+  <si>
+    <t>socdisad_s</t>
+  </si>
+  <si>
+    <t>matdisad_s</t>
+  </si>
+  <si>
+    <t>socdisad_n</t>
+  </si>
+  <si>
+    <t>matdisad_n</t>
   </si>
 </sst>
 </file>
@@ -916,16 +944,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9294277B-21A7-43CE-8531-93B2C9E785B5}">
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:E16"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -933,13 +961,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
         <v>7</v>
@@ -948,7 +976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -956,22 +984,22 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-2</v>
-      </c>
-      <c r="D2">
-        <v>3.3075009999999998</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
+        <v>-0.1575404</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>3.2543859999999998</v>
+        <v>-0.20573649999999999</v>
       </c>
       <c r="G2">
-        <v>3.360617</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.10934430000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -979,22 +1007,22 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>-2</v>
-      </c>
-      <c r="D3">
-        <v>3.4236140000000002</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
+        <v>0.20159469999999999</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>3.3363070000000001</v>
+        <v>0.1445901</v>
       </c>
       <c r="G3">
-        <v>3.5109210000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.25859929999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1002,22 +1030,22 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>-2</v>
-      </c>
-      <c r="D4">
-        <v>3.3906540000000001</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
+        <v>5.0006799999999997E-2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>3.2583440000000001</v>
+        <v>-4.5976400000000001E-2</v>
       </c>
       <c r="G4">
-        <v>3.5229629999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.14599000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1025,22 +1053,22 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>-1</v>
-      </c>
-      <c r="D5">
-        <v>3.4118170000000001</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
+        <v>-0.17006779999999999</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>3.3758189999999999</v>
+        <v>-0.2166633</v>
       </c>
       <c r="G5">
-        <v>3.447816</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.1234722</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1048,22 +1076,22 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>-1</v>
-      </c>
-      <c r="D6">
-        <v>3.4547780000000001</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
+        <v>0.60125490000000004</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>3.3970009999999999</v>
+        <v>0.51456869999999999</v>
       </c>
       <c r="G6">
-        <v>3.5125549999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.68794109999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1071,22 +1099,22 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>-1</v>
-      </c>
-      <c r="D7">
-        <v>3.47167</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
+        <v>0.26294339999999999</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>3.389154</v>
+        <v>0.1734646</v>
       </c>
       <c r="G7">
-        <v>3.5541849999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.35242210000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1094,22 +1122,22 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>3.516133</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
+        <v>0.168848</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>3.4890840000000001</v>
+        <v>1.3374999999999999E-3</v>
       </c>
       <c r="G8">
-        <v>3.543183</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.33635860000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1117,22 +1145,22 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>3.4859420000000001</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
+        <v>0.2597988</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>3.4460709999999999</v>
+        <v>5.15527E-2</v>
       </c>
       <c r="G9">
-        <v>3.5258129999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.46804499999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1140,22 +1168,22 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>3.5526849999999999</v>
-      </c>
-      <c r="E10" t="s">
-        <v>15</v>
+        <v>0.16188089999999999</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
       </c>
       <c r="F10">
-        <v>3.493458</v>
+        <v>-0.1379842</v>
       </c>
       <c r="G10">
-        <v>3.6119129999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.46174609999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1163,22 +1191,22 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>3.6204489999999998</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
+        <v>-0.32391370000000003</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>3.586856</v>
+        <v>-0.43747659999999999</v>
       </c>
       <c r="G11">
-        <v>3.6540430000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.2103508</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1186,22 +1214,22 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>3.5171060000000001</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
+        <v>-4.4339000000000002E-3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
       </c>
       <c r="F12">
-        <v>3.4683519999999999</v>
+        <v>-0.1608444</v>
       </c>
       <c r="G12">
-        <v>3.5658599999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.15197649999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1209,22 +1237,22 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>3.6337009999999998</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
+        <v>0.4473724</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
       </c>
       <c r="F13">
-        <v>3.5465059999999999</v>
+        <v>0.17822170000000001</v>
       </c>
       <c r="G13">
-        <v>3.7208969999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.71652309999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1232,22 +1260,22 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>3.7247650000000001</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
+        <v>-0.14345369999999999</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
       </c>
       <c r="F14">
-        <v>3.6749010000000002</v>
+        <v>-0.18567629999999999</v>
       </c>
       <c r="G14">
-        <v>3.7746300000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.101231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1255,22 +1283,22 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>3.54827</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
+        <v>0.16428200000000001</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
       </c>
       <c r="F15">
-        <v>3.4727709999999998</v>
+        <v>0.1049649</v>
       </c>
       <c r="G15">
-        <v>3.6237689999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.2235992</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1278,19 +1306,88 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <v>3.7147169999999998</v>
-      </c>
-      <c r="E16" t="s">
-        <v>15</v>
+        <v>0.23916599999999999</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>3.5765349999999998</v>
+        <v>0.14490220000000001</v>
       </c>
       <c r="G16">
-        <v>3.8528989999999999</v>
+        <v>0.3334298</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>-0.32920450000000001</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>-0.46111930000000001</v>
+      </c>
+      <c r="G17">
+        <v>-0.19728970000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>1.0044979999999999</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <v>0.84139989999999998</v>
+      </c>
+      <c r="G18">
+        <v>1.1675960000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>0.12612799999999999</v>
+      </c>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>-7.9753599999999994E-2</v>
+      </c>
+      <c r="G19">
+        <v>0.33200970000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1299,16 +1396,399 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>-2</v>
+      </c>
+      <c r="D2">
+        <v>3.3075009999999998</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>3.249225</v>
+      </c>
+      <c r="G2">
+        <v>3.3657780000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>-2</v>
+      </c>
+      <c r="D3">
+        <v>3.4236140000000002</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>3.327823</v>
+      </c>
+      <c r="G3">
+        <v>3.5194049999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>-2</v>
+      </c>
+      <c r="D4">
+        <v>3.3906540000000001</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>3.2454860000000001</v>
+      </c>
+      <c r="G4">
+        <v>3.5358209999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5">
+        <v>3.4118170000000001</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>3.3723209999999999</v>
+      </c>
+      <c r="G5">
+        <v>3.451314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>3.4547780000000001</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>3.3913869999999999</v>
+      </c>
+      <c r="G6">
+        <v>3.5181689999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>-1</v>
+      </c>
+      <c r="D7">
+        <v>3.47167</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>3.381135</v>
+      </c>
+      <c r="G7">
+        <v>3.5622039999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>3.516133</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>3.486456</v>
+      </c>
+      <c r="G8">
+        <v>3.545811</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>3.4859420000000001</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>3.4421970000000002</v>
+      </c>
+      <c r="G9">
+        <v>3.529687</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>3.5526849999999999</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>3.4877030000000002</v>
+      </c>
+      <c r="G10">
+        <v>3.6176680000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>3.6204489999999998</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>3.5835919999999999</v>
+      </c>
+      <c r="G11">
+        <v>3.6573069999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>3.5171060000000001</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>3.4636140000000002</v>
+      </c>
+      <c r="G12">
+        <v>3.5705979999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>3.6337009999999998</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>3.538033</v>
+      </c>
+      <c r="G13">
+        <v>3.7293690000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>3.7247650000000001</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>3.6700550000000001</v>
+      </c>
+      <c r="G14">
+        <v>3.7794759999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>3.54827</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>3.4654349999999998</v>
+      </c>
+      <c r="G15">
+        <v>3.6311049999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>3.7147169999999998</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>3.5631080000000002</v>
+      </c>
+      <c r="G16">
+        <v>3.8663259999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0E4540-9F28-4960-BBA8-2C1C27FB2A40}">
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1337,7 +1817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1360,13 +1840,13 @@
         <v>11</v>
       </c>
       <c r="H2">
-        <v>3.30925</v>
+        <v>3.300195</v>
       </c>
       <c r="I2">
-        <v>3.495622</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.504677</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1389,13 +1869,13 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <v>2.9414359999999999</v>
+        <v>2.9191099999999999</v>
       </c>
       <c r="I3">
-        <v>3.4009429999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4232689999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1418,13 +1898,13 @@
         <v>11</v>
       </c>
       <c r="H4">
-        <v>2.764929</v>
+        <v>2.7418529999999999</v>
       </c>
       <c r="I4">
-        <v>3.2396280000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.262705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1447,13 +1927,13 @@
         <v>11</v>
       </c>
       <c r="H5">
-        <v>3.490796</v>
+        <v>3.48522</v>
       </c>
       <c r="I5">
-        <v>3.6055679999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6111439999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1476,13 +1956,13 @@
         <v>11</v>
       </c>
       <c r="H6">
-        <v>3.1891829999999999</v>
+        <v>3.1749770000000002</v>
       </c>
       <c r="I6">
-        <v>3.4815589999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.495765</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1505,13 +1985,13 @@
         <v>11</v>
       </c>
       <c r="H7">
-        <v>3.1202450000000002</v>
+        <v>3.104203</v>
       </c>
       <c r="I7">
-        <v>3.45031</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4663520000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1534,13 +2014,13 @@
         <v>11</v>
       </c>
       <c r="H8">
-        <v>3.6571229999999999</v>
+        <v>3.6535470000000001</v>
       </c>
       <c r="I8">
-        <v>3.7307329999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.7343090000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1563,13 +2043,13 @@
         <v>11</v>
       </c>
       <c r="H9">
-        <v>3.4057810000000002</v>
+        <v>3.3966690000000002</v>
       </c>
       <c r="I9">
-        <v>3.593324</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.602436</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1592,13 +2072,13 @@
         <v>11</v>
       </c>
       <c r="H10">
-        <v>3.4418890000000002</v>
+        <v>3.429608</v>
       </c>
       <c r="I10">
-        <v>3.6946629999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.706944</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1621,13 +2101,13 @@
         <v>11</v>
       </c>
       <c r="H11">
-        <v>3.7861199999999999</v>
+        <v>3.7809159999999999</v>
       </c>
       <c r="I11">
-        <v>3.8932280000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.8984320000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1650,13 +2130,13 @@
         <v>11</v>
       </c>
       <c r="H12">
-        <v>3.5410439999999999</v>
+        <v>3.5291220000000001</v>
       </c>
       <c r="I12">
-        <v>3.7864239999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.798346</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1679,13 +2159,13 @@
         <v>11</v>
       </c>
       <c r="H13">
-        <v>3.7011240000000001</v>
+        <v>3.686534</v>
       </c>
       <c r="I13">
-        <v>4.0014250000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0160150000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1708,13 +2188,13 @@
         <v>11</v>
       </c>
       <c r="H14">
-        <v>3.8969130000000001</v>
+        <v>3.8883130000000001</v>
       </c>
       <c r="I14">
-        <v>4.0739270000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0825269999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1737,13 +2217,13 @@
         <v>11</v>
       </c>
       <c r="H15">
-        <v>3.6275409999999999</v>
+        <v>3.6080700000000001</v>
       </c>
       <c r="I15">
-        <v>4.0282900000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0477610000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1766,13 +2246,13 @@
         <v>11</v>
       </c>
       <c r="H16">
-        <v>3.9175949999999999</v>
+        <v>3.8965360000000002</v>
       </c>
       <c r="I16">
-        <v>4.3509510000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.3720100000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1795,13 +2275,13 @@
         <v>11</v>
       </c>
       <c r="H17">
-        <v>2.882285</v>
+        <v>2.8717739999999998</v>
       </c>
       <c r="I17">
-        <v>3.098614</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.109124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1824,13 +2304,13 @@
         <v>15</v>
       </c>
       <c r="H18">
-        <v>3.0097809999999998</v>
+        <v>2.9965769999999998</v>
       </c>
       <c r="I18">
-        <v>3.2815500000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.2947540000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1853,13 +2333,13 @@
         <v>15</v>
       </c>
       <c r="H19">
-        <v>3.2473649999999998</v>
+        <v>3.2343060000000001</v>
       </c>
       <c r="I19">
-        <v>3.5160680000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5291269999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1882,13 +2362,13 @@
         <v>11</v>
       </c>
       <c r="H20">
-        <v>3.1011700000000002</v>
+        <v>3.0949450000000001</v>
       </c>
       <c r="I20">
-        <v>3.2292800000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.2355040000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1911,13 +2391,13 @@
         <v>15</v>
       </c>
       <c r="H21">
-        <v>3.1513179999999998</v>
+        <v>3.1430449999999999</v>
       </c>
       <c r="I21">
-        <v>3.3216100000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3298830000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1940,13 +2420,13 @@
         <v>15</v>
       </c>
       <c r="H22">
-        <v>3.3566859999999998</v>
+        <v>3.347839</v>
       </c>
       <c r="I22">
-        <v>3.5387140000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.547561</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1969,13 +2449,13 @@
         <v>11</v>
       </c>
       <c r="H23">
-        <v>3.2871600000000001</v>
+        <v>3.282025</v>
       </c>
       <c r="I23">
-        <v>3.3928410000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3979759999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1998,13 +2478,13 @@
         <v>15</v>
       </c>
       <c r="H24">
-        <v>3.269037</v>
+        <v>3.2633800000000002</v>
       </c>
       <c r="I24">
-        <v>3.3854880000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3911449999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2027,13 +2507,13 @@
         <v>15</v>
       </c>
       <c r="H25">
-        <v>3.4255499999999999</v>
+        <v>3.4169860000000001</v>
       </c>
       <c r="I25">
-        <v>3.601817</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6103809999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2056,13 +2536,13 @@
         <v>11</v>
       </c>
       <c r="H26">
-        <v>3.4266450000000002</v>
+        <v>3.4180820000000001</v>
       </c>
       <c r="I26">
-        <v>3.6029070000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6114700000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2085,13 +2565,13 @@
         <v>15</v>
       </c>
       <c r="H27">
-        <v>3.3350810000000002</v>
+        <v>3.3270179999999998</v>
       </c>
       <c r="I27">
-        <v>3.5010409999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5091039999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2114,13 +2594,13 @@
         <v>15</v>
       </c>
       <c r="H28">
-        <v>3.4512049999999999</v>
+        <v>3.438723</v>
       </c>
       <c r="I28">
-        <v>3.708129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.7206109999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -2143,13 +2623,13 @@
         <v>11</v>
       </c>
       <c r="H29">
-        <v>3.5516109999999999</v>
+        <v>3.538208</v>
       </c>
       <c r="I29">
-        <v>3.8274919999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.8408959999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -2172,13 +2652,13 @@
         <v>15</v>
       </c>
       <c r="H30">
-        <v>3.3756819999999998</v>
+        <v>3.3627410000000002</v>
       </c>
       <c r="I30">
-        <v>3.6420370000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6549779999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2201,10 +2681,10 @@
         <v>15</v>
       </c>
       <c r="H31">
-        <v>3.4599410000000002</v>
+        <v>3.441897</v>
       </c>
       <c r="I31">
-        <v>3.8313600000000001</v>
+        <v>3.849405</v>
       </c>
     </row>
   </sheetData>
@@ -2213,17 +2693,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6B9039-CBE8-49C0-9D0B-FD71EAE35EE3}">
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2252,7 +2732,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2275,13 +2755,13 @@
         <v>11</v>
       </c>
       <c r="H2">
-        <v>3.3253189999999999</v>
+        <v>3.3178749999999999</v>
       </c>
       <c r="I2">
-        <v>3.4785309999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4859749999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2304,13 +2784,13 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <v>2.9580479999999998</v>
+        <v>2.9351289999999999</v>
       </c>
       <c r="I3">
-        <v>3.4297240000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4526430000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2333,13 +2813,13 @@
         <v>11</v>
       </c>
       <c r="H4">
-        <v>2.8370790000000001</v>
+        <v>2.8120790000000002</v>
       </c>
       <c r="I4">
-        <v>3.3513380000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3763380000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2362,13 +2842,13 @@
         <v>11</v>
       </c>
       <c r="H5">
-        <v>3.4968189999999999</v>
+        <v>3.4921700000000002</v>
       </c>
       <c r="I5">
-        <v>3.5924939999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5971419999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2391,13 +2871,13 @@
         <v>11</v>
       </c>
       <c r="H6">
-        <v>3.1731980000000002</v>
+        <v>3.1583130000000001</v>
       </c>
       <c r="I6">
-        <v>3.4795310000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4944160000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2420,13 +2900,13 @@
         <v>11</v>
       </c>
       <c r="H7">
-        <v>3.1735259999999998</v>
+        <v>3.1574900000000001</v>
       </c>
       <c r="I7">
-        <v>3.5034169999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5194540000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2449,13 +2929,13 @@
         <v>11</v>
       </c>
       <c r="H8">
-        <v>3.6488990000000001</v>
+        <v>3.645159</v>
       </c>
       <c r="I8">
-        <v>3.725876</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.729616</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2478,13 +2958,13 @@
         <v>11</v>
       </c>
       <c r="H9">
-        <v>3.342387</v>
+        <v>3.3310710000000001</v>
       </c>
       <c r="I9">
-        <v>3.5752989999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5866150000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2507,13 +2987,13 @@
         <v>11</v>
       </c>
       <c r="H10">
-        <v>3.454682</v>
+        <v>3.442237</v>
       </c>
       <c r="I10">
-        <v>3.710788</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.723233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2536,13 +3016,13 @@
         <v>11</v>
       </c>
       <c r="H11">
-        <v>3.7714050000000001</v>
+        <v>3.7656999999999998</v>
       </c>
       <c r="I11">
-        <v>3.888833</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.8945379999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2565,13 +3045,13 @@
         <v>11</v>
       </c>
       <c r="H12">
-        <v>3.4303089999999998</v>
+        <v>3.414663</v>
       </c>
       <c r="I12">
-        <v>3.7523339999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.7679800000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2594,13 +3074,13 @@
         <v>11</v>
       </c>
       <c r="H13">
-        <v>3.643456</v>
+        <v>3.6256210000000002</v>
       </c>
       <c r="I13">
-        <v>4.0105399999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0283759999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2623,13 +3103,13 @@
         <v>11</v>
       </c>
       <c r="H14">
-        <v>3.8823729999999999</v>
+        <v>3.8735810000000002</v>
       </c>
       <c r="I14">
-        <v>4.0633280000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.07212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2652,13 +3132,13 @@
         <v>11</v>
       </c>
       <c r="H15">
-        <v>3.477732</v>
+        <v>3.4538199999999999</v>
       </c>
       <c r="I15">
-        <v>3.9698669999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.993779</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2681,13 +3161,13 @@
         <v>11</v>
       </c>
       <c r="H16">
-        <v>3.79006</v>
+        <v>3.7627329999999999</v>
       </c>
       <c r="I16">
-        <v>4.3524630000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.3797899999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -2710,13 +3190,13 @@
         <v>11</v>
       </c>
       <c r="H17">
-        <v>2.8041149999999999</v>
+        <v>2.7916150000000002</v>
       </c>
       <c r="I17">
-        <v>3.0613999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.0739000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2739,13 +3219,13 @@
         <v>15</v>
       </c>
       <c r="H18">
-        <v>3.0118770000000001</v>
+        <v>3.0006879999999998</v>
       </c>
       <c r="I18">
-        <v>3.242162</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.2533500000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -2768,13 +3248,13 @@
         <v>15</v>
       </c>
       <c r="H19">
-        <v>3.1951420000000001</v>
+        <v>3.1810700000000001</v>
       </c>
       <c r="I19">
-        <v>3.484712</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4987840000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -2797,13 +3277,13 @@
         <v>11</v>
       </c>
       <c r="H20">
-        <v>3.0610919999999999</v>
+        <v>3.0545279999999999</v>
       </c>
       <c r="I20">
-        <v>3.196196</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.2027610000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -2826,13 +3306,13 @@
         <v>15</v>
       </c>
       <c r="H21">
-        <v>3.169432</v>
+        <v>3.1624530000000002</v>
       </c>
       <c r="I21">
-        <v>3.3130630000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3200409999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -2855,13 +3335,13 @@
         <v>15</v>
       </c>
       <c r="H22">
-        <v>3.329653</v>
+        <v>3.319995</v>
       </c>
       <c r="I22">
-        <v>3.528397</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5380549999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -2884,13 +3364,13 @@
         <v>11</v>
       </c>
       <c r="H23">
-        <v>3.2637119999999999</v>
+        <v>3.2578019999999999</v>
       </c>
       <c r="I23">
-        <v>3.3853490000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3912589999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2913,13 +3393,13 @@
         <v>15</v>
       </c>
       <c r="H24">
-        <v>3.309123</v>
+        <v>3.3046180000000001</v>
       </c>
       <c r="I24">
-        <v>3.4018280000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4063319999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2942,13 +3422,13 @@
         <v>15</v>
       </c>
       <c r="H25">
-        <v>3.4317250000000001</v>
+        <v>3.4233289999999998</v>
       </c>
       <c r="I25">
-        <v>3.6045199999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6129159999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2971,13 +3451,13 @@
         <v>11</v>
       </c>
       <c r="H26">
-        <v>3.4022830000000002</v>
+        <v>3.3908040000000002</v>
       </c>
       <c r="I26">
-        <v>3.6385510000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6500300000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3000,13 +3480,13 @@
         <v>15</v>
       </c>
       <c r="H27">
-        <v>3.4046560000000001</v>
+        <v>3.3983349999999999</v>
       </c>
       <c r="I27">
-        <v>3.5347499999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5410710000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3029,13 +3509,13 @@
         <v>15</v>
       </c>
       <c r="H28">
-        <v>3.4900350000000002</v>
+        <v>3.4786480000000002</v>
       </c>
       <c r="I28">
-        <v>3.724405</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.735792</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -3058,13 +3538,13 @@
         <v>11</v>
       </c>
       <c r="H29">
-        <v>3.5283310000000001</v>
+        <v>3.5100660000000001</v>
       </c>
       <c r="I29">
-        <v>3.9042759999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.9225409999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -3087,13 +3567,13 @@
         <v>15</v>
       </c>
       <c r="H30">
-        <v>3.4771369999999999</v>
+        <v>3.4667590000000001</v>
       </c>
       <c r="I30">
-        <v>3.690725</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.7011029999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -3116,10 +3596,10 @@
         <v>15</v>
       </c>
       <c r="H31">
-        <v>3.5269729999999999</v>
+        <v>3.5105179999999998</v>
       </c>
       <c r="I31">
-        <v>3.8656630000000001</v>
+        <v>3.8821180000000002</v>
       </c>
     </row>
   </sheetData>
@@ -3127,15 +3607,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFB957D-785C-4A54-8A36-EE5236BB7762}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3164,7 +3646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3187,13 +3669,13 @@
         <v>11</v>
       </c>
       <c r="H2">
-        <v>3.2156509999999998</v>
+        <v>3.2053289999999999</v>
       </c>
       <c r="I2">
-        <v>3.428112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.438434</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3216,13 +3698,13 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <v>2.975562</v>
+        <v>2.9591630000000002</v>
       </c>
       <c r="I3">
-        <v>3.313097</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3294969999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3245,13 +3727,13 @@
         <v>11</v>
       </c>
       <c r="H4">
-        <v>2.8315610000000002</v>
+        <v>2.807077</v>
       </c>
       <c r="I4">
-        <v>3.335261</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3597459999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3274,13 +3756,13 @@
         <v>11</v>
       </c>
       <c r="H5">
-        <v>3.4232040000000001</v>
+        <v>3.4167860000000001</v>
       </c>
       <c r="I5">
-        <v>3.555291</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.561709</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3303,13 +3785,13 @@
         <v>11</v>
       </c>
       <c r="H6">
-        <v>3.2027459999999999</v>
+        <v>3.192361</v>
       </c>
       <c r="I6">
-        <v>3.4164970000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4268830000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3332,13 +3814,13 @@
         <v>11</v>
       </c>
       <c r="H7">
-        <v>3.1516999999999999</v>
+        <v>3.1348560000000001</v>
       </c>
       <c r="I7">
-        <v>3.498256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5150999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3361,13 +3843,13 @@
         <v>11</v>
       </c>
       <c r="H8">
-        <v>3.6169009999999999</v>
+        <v>3.6130420000000001</v>
       </c>
       <c r="I8">
-        <v>3.6963270000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.700186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3390,13 +3872,13 @@
         <v>11</v>
       </c>
       <c r="H9">
-        <v>3.4051619999999998</v>
+        <v>3.3983840000000001</v>
       </c>
       <c r="I9">
-        <v>3.5446659999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.551444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -3419,13 +3901,13 @@
         <v>11</v>
       </c>
       <c r="H10">
-        <v>3.450793</v>
+        <v>3.4395449999999999</v>
       </c>
       <c r="I10">
-        <v>3.6822940000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.693543</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3448,13 +3930,13 @@
         <v>11</v>
       </c>
       <c r="H11">
-        <v>3.769841</v>
+        <v>3.7645810000000002</v>
       </c>
       <c r="I11">
-        <v>3.8781180000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.8833790000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3477,13 +3959,13 @@
         <v>11</v>
       </c>
       <c r="H12">
-        <v>3.5463369999999999</v>
+        <v>3.5372150000000002</v>
       </c>
       <c r="I12">
-        <v>3.734076</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.7431969999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3506,13 +3988,13 @@
         <v>11</v>
       </c>
       <c r="H13">
-        <v>3.6917230000000001</v>
+        <v>3.6804139999999999</v>
       </c>
       <c r="I13">
-        <v>3.9244979999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.9358070000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -3535,13 +4017,13 @@
         <v>11</v>
       </c>
       <c r="H14">
-        <v>3.8995669999999998</v>
+        <v>3.8906489999999998</v>
       </c>
       <c r="I14">
-        <v>4.0831239999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0920420000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3564,13 +4046,13 @@
         <v>11</v>
       </c>
       <c r="H15">
-        <v>3.652984</v>
+        <v>3.6381640000000002</v>
       </c>
       <c r="I15">
-        <v>3.9580129999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.9728330000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3593,13 +4075,13 @@
         <v>11</v>
       </c>
       <c r="H16">
-        <v>3.8751289999999998</v>
+        <v>3.8581650000000001</v>
       </c>
       <c r="I16">
-        <v>4.2242240000000004</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.2411880000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -3622,13 +4104,13 @@
         <v>11</v>
       </c>
       <c r="H17">
-        <v>3.0117340000000001</v>
+        <v>3.0031479999999999</v>
       </c>
       <c r="I17">
-        <v>3.1884570000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.197044</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3651,13 +4133,13 @@
         <v>15</v>
       </c>
       <c r="H18">
-        <v>3.0087739999999998</v>
+        <v>2.9932310000000002</v>
       </c>
       <c r="I18">
-        <v>3.3287</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3442430000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -3680,13 +4162,13 @@
         <v>15</v>
       </c>
       <c r="H19">
-        <v>3.2239599999999999</v>
+        <v>3.2080609999999998</v>
       </c>
       <c r="I19">
-        <v>3.5510269999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.566926</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -3709,13 +4191,13 @@
         <v>11</v>
       </c>
       <c r="H20">
-        <v>3.2040329999999999</v>
+        <v>3.1984530000000002</v>
       </c>
       <c r="I20">
-        <v>3.3188710000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3244509999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -3738,13 +4220,13 @@
         <v>15</v>
       </c>
       <c r="H21">
-        <v>3.1353059999999999</v>
+        <v>3.1253950000000001</v>
       </c>
       <c r="I21">
-        <v>3.339299</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3492099999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -3767,13 +4249,13 @@
         <v>15</v>
       </c>
       <c r="H22">
-        <v>3.3449080000000002</v>
+        <v>3.3345850000000001</v>
       </c>
       <c r="I22">
-        <v>3.5572629999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.5675870000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -3796,13 +4278,13 @@
         <v>11</v>
       </c>
       <c r="H23">
-        <v>3.3758509999999999</v>
+        <v>3.371289</v>
       </c>
       <c r="I23">
-        <v>3.4697650000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.4743270000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3825,13 +4307,13 @@
         <v>15</v>
       </c>
       <c r="H24">
-        <v>3.2299220000000002</v>
+        <v>3.2225429999999999</v>
       </c>
       <c r="I24">
-        <v>3.3818139999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.3891930000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -3854,13 +4336,13 @@
         <v>15</v>
       </c>
       <c r="H25">
-        <v>3.4167040000000002</v>
+        <v>3.4071829999999999</v>
       </c>
       <c r="I25">
-        <v>3.6126529999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6221739999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -3883,13 +4365,13 @@
         <v>11</v>
       </c>
       <c r="H26">
-        <v>3.5168469999999998</v>
+        <v>3.5103059999999999</v>
       </c>
       <c r="I26">
-        <v>3.6514820000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.658023</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3912,13 +4394,13 @@
         <v>15</v>
       </c>
       <c r="H27">
-        <v>3.2663530000000001</v>
+        <v>3.2558509999999998</v>
       </c>
       <c r="I27">
-        <v>3.4825149999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.493017</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3941,13 +4423,13 @@
         <v>15</v>
       </c>
       <c r="H28">
-        <v>3.4308879999999999</v>
+        <v>3.4165670000000001</v>
       </c>
       <c r="I28">
-        <v>3.725654</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.7399740000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -3970,13 +4452,13 @@
         <v>11</v>
       </c>
       <c r="H29">
-        <v>3.6441439999999998</v>
+        <v>3.6342940000000001</v>
       </c>
       <c r="I29">
-        <v>3.8468969999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.8567469999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -3999,13 +4481,13 @@
         <v>15</v>
       </c>
       <c r="H30">
-        <v>3.275236</v>
+        <v>3.2589350000000001</v>
       </c>
       <c r="I30">
-        <v>3.6107619999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6270639999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -4028,10 +4510,10 @@
         <v>15</v>
       </c>
       <c r="H31">
-        <v>3.4235980000000001</v>
+        <v>3.40239</v>
       </c>
       <c r="I31">
-        <v>3.860128</v>
+        <v>3.8813360000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Margins for race-sex interactions (SRH-AL)
</commit_message>
<xml_diff>
--- a/Margins (Diss Projects 1-2).xlsx
+++ b/Margins (Diss Projects 1-2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlb15b\Desktop\STATA Data\Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6922B16A-B992-4F8B-A02B-7D089CE9F30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A349A680-D1C3-4CF7-8792-95F5A4B1FFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Disadvantage by Race (Desc)" sheetId="5" r:id="rId1"/>
@@ -18,13 +18,15 @@
     <sheet name="Margins (Total Disad)" sheetId="2" r:id="rId3"/>
     <sheet name="Margins (Material Disad)" sheetId="3" r:id="rId4"/>
     <sheet name="Margins (Social Disad)" sheetId="4" r:id="rId5"/>
+    <sheet name="Margins (SRH by Race-Sex)" sheetId="8" r:id="rId6"/>
+    <sheet name="Margins (AL by Race-Sex)" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="30">
   <si>
     <t>race_eth</t>
   </si>
@@ -99,6 +101,21 @@
   </si>
   <si>
     <t>matdisad_n</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>p &lt; 0.10</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>sex_q</t>
   </si>
 </sst>
 </file>
@@ -947,7 +964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9294277B-21A7-43CE-8531-93B2C9E785B5}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -1400,7 +1417,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,10 +1439,10 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1783,7 +1800,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K55" sqref="K55"/>
+      <selection activeCell="H1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,10 +1828,10 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2698,7 +2715,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="H1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2726,10 +2743,10 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3612,7 +3629,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="H1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3640,10 +3657,10 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4519,4 +4536,1834 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A227BD-61E2-4F4B-8F76-4D7DDAE131D7}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>-2</v>
+      </c>
+      <c r="F2">
+        <v>3.296789</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <v>3.2193550000000002</v>
+      </c>
+      <c r="I2">
+        <v>3.3742239999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>-2</v>
+      </c>
+      <c r="F3">
+        <v>3.3205589999999998</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>3.2490199999999998</v>
+      </c>
+      <c r="I3">
+        <v>3.3920979999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>-2</v>
+      </c>
+      <c r="F4">
+        <v>3.3590960000000001</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>3.206359</v>
+      </c>
+      <c r="I4">
+        <v>3.5118339999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>-2</v>
+      </c>
+      <c r="F5">
+        <v>3.486774</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>3.3616380000000001</v>
+      </c>
+      <c r="I5">
+        <v>3.61191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>-2</v>
+      </c>
+      <c r="F6">
+        <v>3.4770810000000001</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>3.2135859999999998</v>
+      </c>
+      <c r="I6">
+        <v>3.7405759999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>-2</v>
+      </c>
+      <c r="F7">
+        <v>3.3226450000000001</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>3.1872880000000001</v>
+      </c>
+      <c r="I7">
+        <v>3.458002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+      <c r="F8">
+        <v>3.377065</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>3.3251339999999998</v>
+      </c>
+      <c r="I8">
+        <v>3.4289960000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>-1</v>
+      </c>
+      <c r="F9">
+        <v>3.4491770000000002</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9">
+        <v>3.4038409999999999</v>
+      </c>
+      <c r="I9">
+        <v>3.4945140000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+      <c r="F10">
+        <v>3.3894739999999999</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10">
+        <v>3.2997749999999999</v>
+      </c>
+      <c r="I10">
+        <v>3.4791720000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>-1</v>
+      </c>
+      <c r="F11">
+        <v>3.5175230000000002</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>3.4331520000000002</v>
+      </c>
+      <c r="I11">
+        <v>3.6018940000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>-1</v>
+      </c>
+      <c r="F12">
+        <v>3.493249</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12">
+        <v>3.3328289999999998</v>
+      </c>
+      <c r="I12">
+        <v>3.6536680000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>-1</v>
+      </c>
+      <c r="F13">
+        <v>3.4620090000000001</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13">
+        <v>3.3800819999999998</v>
+      </c>
+      <c r="I13">
+        <v>3.5439349999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>3.4573399999999999</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14">
+        <v>3.4153769999999999</v>
+      </c>
+      <c r="I14">
+        <v>3.499304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>3.5777960000000002</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15">
+        <v>3.5467849999999999</v>
+      </c>
+      <c r="I15">
+        <v>3.608806</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>3.419851</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>3.3602180000000001</v>
+      </c>
+      <c r="I16">
+        <v>3.4794839999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>3.5482719999999999</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <v>3.4925839999999999</v>
+      </c>
+      <c r="I17">
+        <v>3.603961</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>3.509417</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18">
+        <v>3.4064040000000002</v>
+      </c>
+      <c r="I18">
+        <v>3.6124290000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>3.601372</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19">
+        <v>3.5344410000000002</v>
+      </c>
+      <c r="I19">
+        <v>3.6683029999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>3.5376159999999999</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20">
+        <v>3.48115</v>
+      </c>
+      <c r="I20">
+        <v>3.5940820000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>3.7064140000000001</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21">
+        <v>3.6635589999999998</v>
+      </c>
+      <c r="I21">
+        <v>3.7492700000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>3.4502280000000001</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22">
+        <v>3.3509340000000001</v>
+      </c>
+      <c r="I22">
+        <v>3.5495220000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>3.5790220000000001</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23">
+        <v>3.5189620000000001</v>
+      </c>
+      <c r="I23">
+        <v>3.639081</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>3.5255839999999998</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24">
+        <v>3.3704679999999998</v>
+      </c>
+      <c r="I24">
+        <v>3.6806999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>3.7407360000000001</v>
+      </c>
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25">
+        <v>3.6329120000000001</v>
+      </c>
+      <c r="I25">
+        <v>3.84856</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>3.6178910000000002</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26">
+        <v>3.5343490000000002</v>
+      </c>
+      <c r="I26">
+        <v>3.7014330000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>3.8350330000000001</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27">
+        <v>3.7666200000000001</v>
+      </c>
+      <c r="I27">
+        <v>3.9034450000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>3.4806050000000002</v>
+      </c>
+      <c r="G28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28">
+        <v>3.3164229999999999</v>
+      </c>
+      <c r="I28">
+        <v>3.644787</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>3.6097709999999998</v>
+      </c>
+      <c r="G29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29">
+        <v>3.5168379999999999</v>
+      </c>
+      <c r="I29">
+        <v>3.7027030000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>3.5417519999999998</v>
+      </c>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30">
+        <v>3.2846880000000001</v>
+      </c>
+      <c r="I30">
+        <v>3.798816</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>3.880099</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31">
+        <v>3.7123200000000001</v>
+      </c>
+      <c r="I31">
+        <v>4.0478779999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E5EA93-4C37-4F80-9262-603EFCA6D4B2}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>-2</v>
+      </c>
+      <c r="F2">
+        <v>2.7191779999999999</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>2.364233</v>
+      </c>
+      <c r="I2">
+        <v>3.0741230000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>-2</v>
+      </c>
+      <c r="F3">
+        <v>3.2288019999999999</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>3.0170119999999998</v>
+      </c>
+      <c r="I3">
+        <v>3.4405920000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>-2</v>
+      </c>
+      <c r="F4">
+        <v>3.3265570000000002</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4">
+        <v>2.7185839999999999</v>
+      </c>
+      <c r="I4">
+        <v>3.9345300000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>-2</v>
+      </c>
+      <c r="F5">
+        <v>3.3189700000000002</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>2.6684540000000001</v>
+      </c>
+      <c r="I5">
+        <v>3.9694859999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>-2</v>
+      </c>
+      <c r="F6">
+        <v>2.904833</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>2.1628189999999998</v>
+      </c>
+      <c r="I6">
+        <v>3.6468470000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>-2</v>
+      </c>
+      <c r="F7">
+        <v>2.5334889999999999</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>1.880514</v>
+      </c>
+      <c r="I7">
+        <v>3.186464</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+      <c r="F8">
+        <v>2.6883180000000002</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>2.4756589999999998</v>
+      </c>
+      <c r="I8">
+        <v>2.9009770000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>-1</v>
+      </c>
+      <c r="F9">
+        <v>3.0193189999999999</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9">
+        <v>2.883165</v>
+      </c>
+      <c r="I9">
+        <v>3.1554730000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+      <c r="F10">
+        <v>3.022408</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10">
+        <v>2.6166749999999999</v>
+      </c>
+      <c r="I10">
+        <v>3.4281410000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>-1</v>
+      </c>
+      <c r="F11">
+        <v>3.1624970000000001</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>2.7549809999999999</v>
+      </c>
+      <c r="I11">
+        <v>3.5700129999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>-1</v>
+      </c>
+      <c r="F12">
+        <v>2.65707</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12">
+        <v>2.2206700000000001</v>
+      </c>
+      <c r="I12">
+        <v>3.0934689999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>-1</v>
+      </c>
+      <c r="F13">
+        <v>2.5882489999999998</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <v>2.1766540000000001</v>
+      </c>
+      <c r="I13">
+        <v>2.9998429999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>2.6574580000000001</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14">
+        <v>2.535803</v>
+      </c>
+      <c r="I14">
+        <v>2.7791130000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>2.8098359999999998</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15">
+        <v>2.692348</v>
+      </c>
+      <c r="I15">
+        <v>2.9273250000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>2.7182590000000002</v>
+      </c>
+      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16">
+        <v>2.4457949999999999</v>
+      </c>
+      <c r="I16">
+        <v>2.990723</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>3.006024</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <v>2.777272</v>
+      </c>
+      <c r="I17">
+        <v>3.2347769999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>2.4093059999999999</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18">
+        <v>2.1650260000000001</v>
+      </c>
+      <c r="I18">
+        <v>2.6535869999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>2.643008</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19">
+        <v>2.3397160000000001</v>
+      </c>
+      <c r="I19">
+        <v>2.9462999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>2.626598</v>
+      </c>
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20">
+        <v>2.44028</v>
+      </c>
+      <c r="I20">
+        <v>2.812916</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>2.6003530000000001</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21">
+        <v>2.4252769999999999</v>
+      </c>
+      <c r="I21">
+        <v>2.7754300000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>2.41411</v>
+      </c>
+      <c r="G22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22">
+        <v>2.1002900000000002</v>
+      </c>
+      <c r="I22">
+        <v>2.7279309999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>2.8495520000000001</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23">
+        <v>2.563291</v>
+      </c>
+      <c r="I23">
+        <v>3.135812</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>2.161543</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24">
+        <v>1.7637119999999999</v>
+      </c>
+      <c r="I24">
+        <v>2.559374</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>2.6977679999999999</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25">
+        <v>2.2571949999999998</v>
+      </c>
+      <c r="I25">
+        <v>3.138341</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>2.5957379999999999</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26">
+        <v>2.2717520000000002</v>
+      </c>
+      <c r="I26">
+        <v>2.919724</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>2.3908710000000002</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27">
+        <v>2.1280350000000001</v>
+      </c>
+      <c r="I27">
+        <v>2.6537060000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>2.1099619999999999</v>
+      </c>
+      <c r="G28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28">
+        <v>1.6227659999999999</v>
+      </c>
+      <c r="I28">
+        <v>2.5971570000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>2.693079</v>
+      </c>
+      <c r="G29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29">
+        <v>2.1881810000000002</v>
+      </c>
+      <c r="I29">
+        <v>3.1979769999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>1.91378</v>
+      </c>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30">
+        <v>1.216475</v>
+      </c>
+      <c r="I30">
+        <v>2.6110850000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>2.7525270000000002</v>
+      </c>
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31">
+        <v>2.0627689999999999</v>
+      </c>
+      <c r="I31">
+        <v>3.442285</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>